<commit_message>
add emota test results for en, de models
</commit_message>
<xml_diff>
--- a/problem_statement_claim/Metadata (Paper, Model repos, tested results).xlsx
+++ b/problem_statement_claim/Metadata (Paper, Model repos, tested results).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FYP\CodeBase\GitHub\Multilingual-Speech-Emotion-Recognition\problem_statement_claim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA0B6B7-0CBD-4DA6-B54E-29E1BF5CFC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3CC2B1-8E93-4800-BC24-56C6BEFF6CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>Language</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t xml:space="preserve">1D-CNN-LSTM-GRU-English model </t>
+  </si>
+  <si>
+    <t>Tamil</t>
+  </si>
+  <si>
+    <t>EmoTa</t>
   </si>
 </sst>
 </file>
@@ -172,7 +178,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -517,6 +523,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -528,36 +564,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -565,24 +571,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -702,6 +690,25 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -716,16 +723,15 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -741,14 +747,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA7548E0-74F8-4B55-B82E-DA9A24D36320}" name="Table1" displayName="Table1" ref="A1:E7" totalsRowShown="0" headerRowDxfId="0" dataDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA7548E0-74F8-4B55-B82E-DA9A24D36320}" name="Table1" displayName="Table1" ref="A1:E7" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A1:E7" xr:uid="{DA7548E0-74F8-4B55-B82E-DA9A24D36320}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6EF82C10-3C26-42AC-B080-007A5FADFEA9}" name="Language" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{B8DF9244-F8FE-42B6-8DA4-654898ED36E4}" name="Dataset" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C7DC20C9-760A-4E9D-B012-DD6118C94007}" name="PaperLink" dataDxfId="3" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{C7CB4F82-D621-494A-B18B-9738C52767EE}" name="Accuracy" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{F2D27E55-8E28-4640-A34F-6641C8CC5A1D}" name="Model’s link" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{6EF82C10-3C26-42AC-B080-007A5FADFEA9}" name="Language" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{B8DF9244-F8FE-42B6-8DA4-654898ED36E4}" name="Dataset" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{C7DC20C9-760A-4E9D-B012-DD6118C94007}" name="PaperLink" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{C7CB4F82-D621-494A-B18B-9738C52767EE}" name="Accuracy" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{F2D27E55-8E28-4640-A34F-6641C8CC5A1D}" name="Model’s link" dataDxfId="0" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1169,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648B92E0-0F11-471E-BB8D-F2E31B075FC5}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1186,14 +1192,14 @@
     <col min="14" max="14" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:15" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="18"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="13" t="s">
         <v>20</v>
       </c>
@@ -1227,278 +1233,294 @@
       <c r="N1" s="13" t="s">
         <v>27</v>
       </c>
+      <c r="O1" s="13" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16"/>
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="1:15" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="26"/>
+      <c r="B2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="16" t="s">
         <v>39</v>
       </c>
+      <c r="O2" s="16" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="17">
         <v>0.78700000000000003</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="18">
         <v>0.33</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="18">
         <v>0.42099999999999999</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="18">
         <v>0.39200000000000002</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="18">
         <v>0.53400000000000003</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="18">
         <v>0.496</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="19">
         <v>0.18</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="18">
         <v>0.01</v>
       </c>
-      <c r="J3" s="22">
+      <c r="J3" s="18">
         <v>0.1</v>
       </c>
-      <c r="K3" s="22">
+      <c r="K3" s="18">
         <v>0.16</v>
       </c>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
     </row>
-    <row r="4" spans="1:14" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="18">
         <v>0.31</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="18">
         <v>0.46200000000000002</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="17">
         <v>0.63900000000000001</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="18">
         <v>0.38</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="18">
         <v>0.51</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="18">
         <v>0.48799999999999999</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="18">
         <v>0.25</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="18">
         <v>0.33</v>
       </c>
-      <c r="K4" s="22">
+      <c r="K4" s="18">
         <v>0.19</v>
       </c>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
     </row>
-    <row r="5" spans="1:14" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26">
+      <c r="B5" s="21"/>
+      <c r="C5" s="22">
         <v>0.128</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="23">
         <v>0.23</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="23">
         <v>0.111</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="23">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="23">
         <v>0.08</v>
       </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
     </row>
-    <row r="6" spans="1:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="20">
         <v>0.187</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="18">
         <v>0.186</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="18">
         <v>0.17799999999999999</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="17">
         <v>0.97699999999999998</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="18">
         <v>0.21099999999999999</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="18">
         <v>0.16400000000000001</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="18">
         <v>0.15</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="18">
         <v>0.14399999999999999</v>
       </c>
-      <c r="K6" s="22">
+      <c r="K6" s="18">
         <v>0.17799999999999999</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6" s="19">
         <v>0.153</v>
       </c>
-      <c r="M6" s="23">
+      <c r="M6" s="19">
         <v>0.154</v>
       </c>
-      <c r="N6" s="23">
+      <c r="N6" s="19">
         <v>0.16</v>
       </c>
+      <c r="O6" s="19">
+        <v>0.12</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="18">
         <v>0.11700000000000001</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="17">
         <v>0.96199999999999997</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="18">
         <v>0.16400000000000001</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="18">
         <v>0.122</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="18">
         <v>0.26400000000000001</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="20">
         <v>0.183</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="18">
         <v>0.24399999999999999</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="18">
         <v>0.17</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="18">
         <v>0.2</v>
       </c>
-      <c r="K7" s="22">
+      <c r="K7" s="18">
         <v>0.246</v>
       </c>
-      <c r="L7" s="24">
+      <c r="L7" s="20">
         <v>0.127</v>
       </c>
-      <c r="M7" s="24">
+      <c r="M7" s="20">
         <v>0.14000000000000001</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="20">
         <v>0.15</v>
       </c>
+      <c r="O7" s="20">
+        <v>0.25</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="20">
         <v>0.76</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="24">
         <v>0.93</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="18">
         <v>0.95</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="18">
         <v>0.89</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="18">
         <v>0.97</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="18">
         <v>0.86</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="18">
         <v>0.13</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="18">
         <v>0.39</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="18">
         <v>0.82</v>
       </c>
-      <c r="K8" s="22">
+      <c r="K8" s="18">
         <v>0.44</v>
       </c>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>